<commit_message>
Commit by farheen: Work on Inward QC functionality. Code merging i.e. purchase order
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelUploads/Download-Format-Item.xlsx
+++ b/InVanWebApp/ExcelUploads/Download-Format-Item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC7F319-DC8F-446F-B9BB-5DA65C43ED95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40A95E8-2BFE-4A7D-8CEC-74703D3F52E5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Item_Name</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Tomato</t>
-  </si>
-  <si>
     <t>Buy</t>
   </si>
   <si>
@@ -53,6 +50,21 @@
   </si>
   <si>
     <t>TM_0001</t>
+  </si>
+  <si>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>Semi-Finished Good</t>
+  </si>
+  <si>
+    <t>TM_0002</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
   </si>
 </sst>
 </file>
@@ -111,37 +123,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -448,11 +430,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,27 +474,44 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>

<commit_message>
commit by Farheen: Resolved the bugs of PO, indent.
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelUploads/Download-Format-Item.xlsx
+++ b/InVanWebApp/ExcelUploads/Download-Format-Item.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6024DFC3-F120-444D-A9D1-73810F24C124}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA26B10-D0E1-404E-8775-37C2F0DD0EE7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Item_Name</t>
   </si>
@@ -52,19 +52,10 @@
     <t>UnitPrice</t>
   </si>
   <si>
-    <t>Tomato454</t>
-  </si>
-  <si>
-    <t>TM_0001434</t>
-  </si>
-  <si>
-    <t>Ginger5786</t>
-  </si>
-  <si>
-    <t>Sell</t>
-  </si>
-  <si>
-    <t>GIN_hjf</t>
+    <t>Palak</t>
+  </si>
+  <si>
+    <t>PL_0001</t>
   </si>
 </sst>
 </file>
@@ -431,11 +422,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,36 +482,10 @@
         <v>11</v>
       </c>
       <c r="E2" s="2">
-        <v>60.05</v>
-      </c>
-      <c r="F2">
-        <v>4512412</v>
+        <v>20.56</v>
       </c>
       <c r="G2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="2">
-        <v>70.78</v>
-      </c>
-      <c r="F3">
-        <v>451222</v>
-      </c>
-      <c r="G3">
-        <v>20000</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit by Farheen: Code merging and bug fixing.
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelUploads/Download-Format-Item.xlsx
+++ b/InVanWebApp/ExcelUploads/Download-Format-Item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A968228-1AD1-4E29-86B8-6B24E0475FE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EA00C0-E62B-449B-B60E-AF340B3DDCFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Item_Name</t>
   </si>
@@ -43,22 +43,67 @@
     <t>Description</t>
   </si>
   <si>
+    <t>Tomato</t>
+  </si>
+  <si>
     <t>Buy</t>
   </si>
   <si>
     <t>Raw Material</t>
   </si>
   <si>
+    <t>TM_0001</t>
+  </si>
+  <si>
     <t>UnitPrice</t>
   </si>
   <si>
-    <t>Mint leaves</t>
-  </si>
-  <si>
-    <t>Mint_0010</t>
-  </si>
-  <si>
-    <t>Testing</t>
+    <t>Garlic Cloves</t>
+  </si>
+  <si>
+    <t>Fresh Ginger</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Kashmiri chilli powder</t>
+  </si>
+  <si>
+    <t>Sunflower Oil</t>
+  </si>
+  <si>
+    <t>Melon seeds</t>
+  </si>
+  <si>
+    <t>Tomato Paste</t>
+  </si>
+  <si>
+    <t>Sodium Tricitrate</t>
+  </si>
+  <si>
+    <t>GC_0002</t>
+  </si>
+  <si>
+    <t>FG_0003</t>
+  </si>
+  <si>
+    <t>ST_0004</t>
+  </si>
+  <si>
+    <t>KCP_0005</t>
+  </si>
+  <si>
+    <t>SNO_0006</t>
+  </si>
+  <si>
+    <t>MLS_0007</t>
+  </si>
+  <si>
+    <t>TMP_0008</t>
+  </si>
+  <si>
+    <t>ST_0009</t>
   </si>
 </sst>
 </file>
@@ -425,11 +470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -473,25 +518,182 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2">
+        <v>40.049999999999997</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2">
         <v>11</v>
       </c>
-      <c r="E2" s="2">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="G2">
+      <c r="G4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>12</v>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2">
+        <v>70</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2">
+        <v>33</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="2">
+        <v>60</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2">
+        <v>55</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -516,5 +718,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committed by Farheen: Bug fixing
</commit_message>
<xml_diff>
--- a/InVanWebApp/ExcelUploads/Download-Format-Item.xlsx
+++ b/InVanWebApp/ExcelUploads/Download-Format-Item.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EA00C0-E62B-449B-B60E-AF340B3DDCFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DC3796-A366-4CC5-B7AC-910E474A4189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Item_Name</t>
   </si>
@@ -43,74 +43,53 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Tomato</t>
-  </si>
-  <si>
     <t>Buy</t>
   </si>
   <si>
     <t>Raw Material</t>
   </si>
   <si>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>Cumin Seeds</t>
+  </si>
+  <si>
+    <t>Turmeric Powder</t>
+  </si>
+  <si>
+    <t>Kesha Masalo</t>
+  </si>
+  <si>
+    <t>Kasuri Methi</t>
+  </si>
+  <si>
+    <t>Onion</t>
+  </si>
+  <si>
+    <t>TM_0007</t>
+  </si>
+  <si>
+    <t>CS_0002</t>
+  </si>
+  <si>
+    <t>KM_0003</t>
+  </si>
+  <si>
+    <t>ON_0005</t>
+  </si>
+  <si>
+    <t>T_0006</t>
+  </si>
+  <si>
     <t>TM_0001</t>
-  </si>
-  <si>
-    <t>UnitPrice</t>
-  </si>
-  <si>
-    <t>Garlic Cloves</t>
-  </si>
-  <si>
-    <t>Fresh Ginger</t>
-  </si>
-  <si>
-    <t>Salt</t>
-  </si>
-  <si>
-    <t>Kashmiri chilli powder</t>
-  </si>
-  <si>
-    <t>Sunflower Oil</t>
-  </si>
-  <si>
-    <t>Melon seeds</t>
-  </si>
-  <si>
-    <t>Tomato Paste</t>
-  </si>
-  <si>
-    <t>Sodium Tricitrate</t>
-  </si>
-  <si>
-    <t>GC_0002</t>
-  </si>
-  <si>
-    <t>FG_0003</t>
-  </si>
-  <si>
-    <t>ST_0004</t>
-  </si>
-  <si>
-    <t>KCP_0005</t>
-  </si>
-  <si>
-    <t>SNO_0006</t>
-  </si>
-  <si>
-    <t>MLS_0007</t>
-  </si>
-  <si>
-    <t>TMP_0008</t>
-  </si>
-  <si>
-    <t>ST_0009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +104,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -153,12 +144,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,11 +462,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +496,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -517,20 +509,17 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
+      <c r="D2" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="E2" s="2">
-        <v>40.049999999999997</v>
+        <v>45</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -538,19 +527,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -561,16 +550,16 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2">
-        <v>11</v>
+        <v>40.049999999999997</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -581,126 +570,67 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E5" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E6" s="2">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2">
-        <v>32</v>
-      </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" s="2">
-        <v>60</v>
-      </c>
-      <c r="G9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="2">
-        <v>55</v>
-      </c>
-      <c r="G10">
-        <v>100</v>
+        <v>8000</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A1048576">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A12:A1048576 A9 A2:A7">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:E1048576">
+  <conditionalFormatting sqref="D3:D1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">

</xml_diff>